<commit_message>
Adding calculations for velocity, based on Lidar TTC measurements
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenpower/Development/GitHub Projects/SensorFusion-Projects/SensorFusionND-3D-Object-Tracking/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5C7DDF-4DB0-6040-8A90-BB0033E79930}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971C3FAA-D369-324D-BFDC-EED58D9389B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51620" yWindow="7380" windowWidth="38840" windowHeight="17820" xr2:uid="{669A409B-D193-1243-8032-91F302D11FB1}"/>
+    <workbookView xWindow="51620" yWindow="7380" windowWidth="38840" windowHeight="17820" activeTab="1" xr2:uid="{669A409B-D193-1243-8032-91F302D11FB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Manual estimates" sheetId="1" r:id="rId1"/>
+    <sheet name="Lidar TTC Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$2:$H$18</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$H$2:$H$18</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Lidar TTC Analysis'!$J$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Lidar TTC Analysis'!$J$2:$J$19</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Lidar TTC Analysis'!$J$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Lidar TTC Analysis'!$J$2:$J$19</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>d0</t>
   </si>
@@ -62,11 +63,26 @@
   <si>
     <t>ttc (Lidar)</t>
   </si>
+  <si>
+    <t>Lidar points</t>
+  </si>
+  <si>
+    <t>TTC Lidar</t>
+  </si>
+  <si>
+    <t>TTC Camera</t>
+  </si>
+  <si>
+    <t>v0 = d1/TTC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -84,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +116,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,9 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -212,6 +237,20 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,7 +320,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>'Manual estimates'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -340,7 +379,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$18</c:f>
+              <c:f>'Manual estimates'!$H$2:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="17"/>
@@ -547,6 +586,313 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Lidar TTC Analysis'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>v0 = d1/TTC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lidar TTC Analysis'!$J$2:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
+                  <c:v>0.6223145344135973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55283514299907743</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46017232494876986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4802554657346525</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59785309219399474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.62998564800907841</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56918188675794912</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57048087775738821</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66132121060261662</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56212232406351981</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.81140385143385207</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72156950902162609</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.74281433912964656</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82113297688697284</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.71772572368925724</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.7227719246054608</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.81083011858836973</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-559B-3C44-A4BE-5FCAA90C7EF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="408121120"/>
+        <c:axId val="408138448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="408121120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="408138448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="408138448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="408121120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -584,6 +930,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
@@ -1059,6 +1445,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx2"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1084,6 +1986,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE65353E-FB4D-CA40-9A8F-4F1238106A95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C60A64E4-96DB-5C4C-A7C8-EDEE02A20877}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1403,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13025358-868A-C944-AB53-3BECCE31F074}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1415,490 +2358,1071 @@
     <col min="5" max="5" width="7.6640625" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="7">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
         <v>7.91</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>7.85</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <f t="shared" ref="E2:E7" si="0">1/B2</f>
         <v>0.1</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="8">
         <f>(D2*E2)/(C2-D2)</f>
         <v>13.083333333333226</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6">
+      <c r="G2" s="10"/>
+      <c r="H2" s="9">
         <f>(E2)/(C2-D2)</f>
         <v>1.666666666666653</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+      <c r="A3" s="11">
         <v>3</v>
       </c>
-      <c r="B3" s="14">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15">
+      <c r="B3" s="17">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18">
         <v>7.85</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="18">
         <v>7.79</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="17">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="19">
         <f>(D3*E3)/(C3-D3)</f>
         <v>12.983333333333418</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="17">
+      <c r="G3" s="10"/>
+      <c r="H3" s="20">
         <f t="shared" ref="H3:H18" si="1">(E3)/(C3-D3)</f>
         <v>1.6666666666666776</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="7">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="5">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6">
         <v>7.79</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>7.68</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="8">
         <f>(D4*E4)/(C4-D4)</f>
         <v>6.9818181818181619</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6">
+      <c r="G4" s="10"/>
+      <c r="H4" s="9">
         <f t="shared" si="1"/>
         <v>0.90909090909090651</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="11">
         <v>5</v>
       </c>
-      <c r="B5" s="14">
-        <v>10</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" s="17">
+        <v>10</v>
+      </c>
+      <c r="C5" s="18">
         <v>7.68</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="18">
         <v>7.64</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="17">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="19">
         <f>(D5*E5)/(C5-D5)</f>
         <v>19.099999999999984</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="17">
+      <c r="G5" s="10"/>
+      <c r="H5" s="20">
         <f t="shared" si="1"/>
         <v>2.4999999999999978</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="7">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="5">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
         <v>7.64</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>7.58</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="8">
         <f>(D6*E6)/(C6-D6)</f>
         <v>12.633333333333416</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6">
+      <c r="G6" s="10"/>
+      <c r="H6" s="9">
         <f t="shared" si="1"/>
         <v>1.6666666666666776</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="11">
         <v>7</v>
       </c>
-      <c r="B7" s="14">
-        <v>10</v>
-      </c>
-      <c r="C7" s="15">
+      <c r="B7" s="17">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18">
         <v>7.58</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="18">
         <v>7.55</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="17">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="19">
         <f>(D7*E7)/(C7-D7)</f>
         <v>25.166666666666458</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="17">
+      <c r="G7" s="10"/>
+      <c r="H7" s="20">
         <f t="shared" si="1"/>
         <v>3.3333333333333059</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="7">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6">
         <v>7.55</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>7.47</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <f t="shared" ref="E8:E18" si="2">1/B8</f>
         <v>0.1</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="8">
         <f t="shared" ref="F8:F18" si="3">(D8*E8)/(C8-D8)</f>
         <v>9.3374999999999915</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6">
+      <c r="G8" s="10"/>
+      <c r="H8" s="9">
         <f t="shared" si="1"/>
         <v>1.2499999999999989</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="A9" s="11">
         <v>9</v>
       </c>
-      <c r="B9" s="14">
-        <v>10</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="B9" s="17">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18">
         <v>7.47</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="18">
         <v>7.43</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="17">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="19">
         <f t="shared" si="3"/>
         <v>18.574999999999985</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="17">
+      <c r="G9" s="10"/>
+      <c r="H9" s="20">
         <f t="shared" si="1"/>
         <v>2.4999999999999978</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="A10" s="7">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6">
         <v>7.43</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>7.39</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="8">
         <f t="shared" si="3"/>
         <v>18.474999999999984</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6">
+      <c r="G10" s="10"/>
+      <c r="H10" s="9">
         <f t="shared" si="1"/>
         <v>2.4999999999999978</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="A11" s="11">
         <v>11</v>
       </c>
-      <c r="B11" s="14">
-        <v>10</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="17">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18">
         <v>7.39</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="18">
         <v>7.2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="17">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="19">
         <f t="shared" si="3"/>
         <v>3.7894736842105368</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="17">
+      <c r="G11" s="10"/>
+      <c r="H11" s="20">
         <f t="shared" si="1"/>
         <v>0.52631578947368562</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="7">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6">
         <v>7.2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>7.27</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="8">
         <f t="shared" si="3"/>
         <v>-10.385714285714375</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6">
+      <c r="G12" s="10"/>
+      <c r="H12" s="9">
         <f t="shared" si="1"/>
         <v>-1.428571428571441</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+      <c r="A13" s="11">
         <v>13</v>
       </c>
-      <c r="B13" s="14">
-        <v>10</v>
-      </c>
-      <c r="C13" s="15">
+      <c r="B13" s="17">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18">
         <v>7.27</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="18">
         <v>7.19</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="17">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="19">
         <f t="shared" si="3"/>
         <v>8.9875000000000931</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="17">
+      <c r="G13" s="10"/>
+      <c r="H13" s="20">
         <f t="shared" si="1"/>
         <v>1.2500000000000129</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="7">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="5">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6">
         <v>7.19</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>7.13</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="5">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="8">
         <f t="shared" si="3"/>
         <v>11.883333333333237</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="6">
+      <c r="G14" s="10"/>
+      <c r="H14" s="9">
         <f t="shared" si="1"/>
         <v>1.666666666666653</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+      <c r="A15" s="11">
         <v>15</v>
       </c>
-      <c r="B15" s="14">
-        <v>10</v>
-      </c>
-      <c r="C15" s="15">
+      <c r="B15" s="17">
+        <v>10</v>
+      </c>
+      <c r="C15" s="18">
         <v>7.13</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="18">
         <v>7.04</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="17">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="19">
         <f t="shared" si="3"/>
         <v>7.8222222222222353</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="17">
+      <c r="G15" s="10"/>
+      <c r="H15" s="20">
         <f t="shared" si="1"/>
         <v>1.1111111111111129</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="7">
         <v>16</v>
       </c>
-      <c r="B16" s="2">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="B16" s="5">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6">
         <v>7.04</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>6.83</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="5">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="8">
         <f t="shared" si="3"/>
         <v>3.2523809523809533</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="6">
+      <c r="G16" s="10"/>
+      <c r="H16" s="9">
         <f t="shared" si="1"/>
         <v>0.47619047619047628</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+      <c r="A17" s="11">
         <v>17</v>
       </c>
-      <c r="B17" s="14">
-        <v>10</v>
-      </c>
-      <c r="C17" s="15">
+      <c r="B17" s="17">
+        <v>10</v>
+      </c>
+      <c r="C17" s="18">
         <v>6.83</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="18">
         <v>6.9</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="17">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="19">
         <f t="shared" si="3"/>
         <v>-9.8571428571428186</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="17">
+      <c r="G17" s="10"/>
+      <c r="H17" s="20">
         <f t="shared" si="1"/>
         <v>-1.4285714285714228</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="7">
         <v>18</v>
       </c>
-      <c r="B18" s="2">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="B18" s="5">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6">
         <v>6.9</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>6.81</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="5">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="8">
         <f t="shared" si="3"/>
         <v>7.5666666666666043</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="6">
+      <c r="G18" s="10"/>
+      <c r="H18" s="9">
         <f t="shared" si="1"/>
         <v>1.1111111111111021</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D67111-E84E-B84A-82C2-D6023A7617D0}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>340</v>
+      </c>
+      <c r="C2" s="22">
+        <v>12.515599999999999</v>
+      </c>
+      <c r="D2" s="21">
+        <v>15.3278</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>309</v>
+      </c>
+      <c r="C3" s="22">
+        <v>12.6142</v>
+      </c>
+      <c r="D3" s="21">
+        <v>12.763400000000001</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7.91</v>
+      </c>
+      <c r="G3" s="4">
+        <v>7.85</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="23">
+        <f>G3/C3</f>
+        <v>0.6223145344135973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>326</v>
+      </c>
+      <c r="C4" s="22">
+        <v>14.090999999999999</v>
+      </c>
+      <c r="D4" s="21">
+        <v>13.5261</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>7.85</v>
+      </c>
+      <c r="G4" s="4">
+        <v>7.79</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="23">
+        <f t="shared" ref="J4:J19" si="0">G4/C4</f>
+        <v>0.55283514299907743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>322</v>
+      </c>
+      <c r="C5" s="22">
+        <v>16.689399999999999</v>
+      </c>
+      <c r="D5" s="21">
+        <v>13.81</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>7.79</v>
+      </c>
+      <c r="G5" s="4">
+        <v>7.68</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.46017232494876986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>344</v>
+      </c>
+      <c r="C6" s="22">
+        <v>15.908200000000001</v>
+      </c>
+      <c r="D6" s="21">
+        <v>13.0276</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7.68</v>
+      </c>
+      <c r="G6" s="4">
+        <v>7.64</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.4802554657346525</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>352</v>
+      </c>
+      <c r="C7" s="22">
+        <v>12.678699999999999</v>
+      </c>
+      <c r="D7" s="21">
+        <v>11.426</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7.64</v>
+      </c>
+      <c r="G7" s="4">
+        <v>7.58</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.59785309219399474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>317</v>
+      </c>
+      <c r="C8" s="22">
+        <v>11.984400000000001</v>
+      </c>
+      <c r="D8" s="21">
+        <v>12.8408</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7.58</v>
+      </c>
+      <c r="G8" s="4">
+        <v>7.55</v>
+      </c>
+      <c r="H8">
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.62998564800907841</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>312</v>
+      </c>
+      <c r="C9" s="22">
+        <v>13.1241</v>
+      </c>
+      <c r="D9" s="21">
+        <v>13.992100000000001</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>7.55</v>
+      </c>
+      <c r="G9" s="4">
+        <v>7.47</v>
+      </c>
+      <c r="H9">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="23">
+        <f t="shared" si="0"/>
+        <v>0.56918188675794912</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>311</v>
+      </c>
+      <c r="C10" s="22">
+        <v>13.024100000000001</v>
+      </c>
+      <c r="D10" s="21">
+        <v>11.273999999999999</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7.47</v>
+      </c>
+      <c r="G10" s="4">
+        <v>7.43</v>
+      </c>
+      <c r="H10">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.57048087775738821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>286</v>
+      </c>
+      <c r="C11" s="22">
+        <v>11.1746</v>
+      </c>
+      <c r="D11" s="21">
+        <v>35.585000000000001</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7.43</v>
+      </c>
+      <c r="G11" s="4">
+        <v>7.39</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="23">
+        <f t="shared" si="0"/>
+        <v>0.66132121060261662</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>302</v>
+      </c>
+      <c r="C12" s="22">
+        <v>12.8086</v>
+      </c>
+      <c r="D12" s="21">
+        <v>12.776199999999999</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7.39</v>
+      </c>
+      <c r="G12" s="4">
+        <v>7.2</v>
+      </c>
+      <c r="H12">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.56212232406351981</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>302</v>
+      </c>
+      <c r="C13" s="22">
+        <v>8.9597800000000003</v>
+      </c>
+      <c r="D13" s="21">
+        <v>11.583600000000001</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>7.27</v>
+      </c>
+      <c r="H13">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.81140385143385207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>316</v>
+      </c>
+      <c r="C14" s="22">
+        <v>9.9643899999999999</v>
+      </c>
+      <c r="D14" s="21">
+        <v>11.4876</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="G14" s="4">
+        <v>7.19</v>
+      </c>
+      <c r="H14">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.72156950902162609</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>312</v>
+      </c>
+      <c r="C15" s="22">
+        <v>9.59863</v>
+      </c>
+      <c r="D15" s="21">
+        <v>12.2294</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2">
+        <v>7.19</v>
+      </c>
+      <c r="G15" s="4">
+        <v>7.13</v>
+      </c>
+      <c r="H15">
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.74281433912964656</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>289</v>
+      </c>
+      <c r="C16" s="22">
+        <v>8.5735200000000003</v>
+      </c>
+      <c r="D16" s="21">
+        <v>10.225</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <v>7.13</v>
+      </c>
+      <c r="G16" s="4">
+        <v>7.04</v>
+      </c>
+      <c r="H16">
+        <v>0.1</v>
+      </c>
+      <c r="J16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.82113297688697284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>297</v>
+      </c>
+      <c r="C17" s="22">
+        <v>9.5161700000000007</v>
+      </c>
+      <c r="D17" s="21">
+        <v>10.685700000000001</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7.04</v>
+      </c>
+      <c r="G17" s="4">
+        <v>6.83</v>
+      </c>
+      <c r="H17">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.71772572368925724</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>279</v>
+      </c>
+      <c r="C18" s="22">
+        <v>9.5465800000000005</v>
+      </c>
+      <c r="D18" s="21">
+        <v>10.0052</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6.83</v>
+      </c>
+      <c r="G18" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="H18">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.7227719246054608</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>303</v>
+      </c>
+      <c r="C19" s="22">
+        <v>8.3987999999999996</v>
+      </c>
+      <c r="D19" s="21">
+        <v>10.5152</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="G19" s="4">
+        <v>6.81</v>
+      </c>
+      <c r="H19">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.81083011858836973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>